<commit_message>
Updating docs and GH repos example file
</commit_message>
<xml_diff>
--- a/My_GitHub_repos.xlsx
+++ b/My_GitHub_repos.xlsx
@@ -1,133 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\GitHub\personal\work-life\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D18523-F415-489F-88D2-4DCFCDAE82BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Repos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Repo Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Homepage</t>
-  </si>
-  <si>
-    <t>CRA-Starter</t>
-  </si>
-  <si>
-    <t>⚛ My starter template for Create React App projects.</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/CRA-Starter/#/</t>
-  </si>
-  <si>
-    <t>FCC-Front-End-Libraries-Projects</t>
-  </si>
-  <si>
-    <t>My freecodecamp.org Front End Libraries Projects.</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/FCC-Front-End-Libraries-Projects/#/</t>
-  </si>
-  <si>
-    <t>FCC-JavaScript-Algorithms-and-Data-Structures-Projects</t>
-  </si>
-  <si>
-    <t>My freecodecamp.org JavaScript Algorithms and Data Structures Projects.</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/FCC-JavaScript-Algorithms-and-Data-Structures-Projects/#/</t>
-  </si>
-  <si>
-    <t>FCC-Responsive-Web-Design-Projects</t>
-  </si>
-  <si>
-    <t>My freecodecamp.org Responsive Web Design Projects.</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/FCC-Responsive-Web-Design-Projects/index.html</t>
-  </si>
-  <si>
-    <t>github-react-portfolio-template</t>
-  </si>
-  <si>
-    <t>✨A performant, accessible, progressive React portfolio template that uses the GitHub REST API.</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/github-react-portfolio-template/#/</t>
-  </si>
-  <si>
-    <t>mshuber1981</t>
-  </si>
-  <si>
-    <t>My Story</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>My GitHub Portfolio</t>
-  </si>
-  <si>
-    <t>https://www.mikeyhuber.me</t>
-  </si>
-  <si>
-    <t>react-contact-form</t>
-  </si>
-  <si>
-    <t>📩 A simple contact form built with React Bootstrap, and powered by AWS.</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/react-contact-form/</t>
-  </si>
-  <si>
-    <t>work-life</t>
-  </si>
-  <si>
-    <t>⚙ Automating my work life...</t>
-  </si>
-  <si>
-    <t>https://mshuber1981.github.io/work-life/</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,28 +61,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -496,156 +396,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="47.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Repo Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Homepage</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>github-react-portfolio-template</v>
+      </c>
+      <c r="B2" t="str">
+        <v>✨A performant, accessible, progressive React portfolio template that uses the GitHub REST API.</v>
+      </c>
+      <c r="C2" t="str">
+        <v>https://mshuber1981.github.io/github-react-portfolio-template/#/</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>mshuber1981</v>
+      </c>
+      <c r="B3" t="str">
+        <v>My Story</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Portfolio</v>
+      </c>
+      <c r="B4" t="str">
+        <v>My GitHub Portfolio</v>
+      </c>
+      <c r="C4" t="str">
+        <v>https://www.mikeyhuber.me</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>react-contact-form</v>
+      </c>
+      <c r="B5" t="str">
+        <v>📩 A simple contact form built with React Bootstrap, and powered by AWS.</v>
+      </c>
+      <c r="C5" t="str">
+        <v>https://mshuber1981.github.io/react-contact-form/</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>vite-starter</v>
+      </c>
+      <c r="C6" t="str">
+        <v>https://mshuber1981.github.io/vite-starter/</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>work-life</v>
+      </c>
+      <c r="B7" t="str">
+        <v>⚙ Automating my work life...</v>
+      </c>
+      <c r="C7" t="str">
+        <v>https://mshuber1981.github.io/work-life/</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" location="/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C3" r:id="rId4" location="/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C4" r:id="rId6" location="/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C6" r:id="rId10" location="/" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="github-react-portfolio-template"/>
+    <hyperlink ref="C2" r:id="rId2" location="/" display="https://mshuber1981.github.io/github-react-portfolio-template/#/"/>
+    <hyperlink ref="A3" r:id="rId3" display="mshuber1981"/>
+    <hyperlink ref="A4" r:id="rId4" display="Portfolio"/>
+    <hyperlink ref="C4" r:id="rId5" display="https://www.mikeyhuber.me"/>
+    <hyperlink ref="A5" r:id="rId6" display="react-contact-form"/>
+    <hyperlink ref="C5" r:id="rId7" display="https://mshuber1981.github.io/react-contact-form/"/>
+    <hyperlink ref="A6" r:id="rId8" display="vite-starter"/>
+    <hyperlink ref="C6" r:id="rId9" display="https://mshuber1981.github.io/vite-starter/"/>
+    <hyperlink ref="A7" r:id="rId10" display="work-life"/>
+    <hyperlink ref="C7" r:id="rId11" display="https://mshuber1981.github.io/work-life/"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;22&amp;KFF8939 RESTRICTED</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:C10" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>